<commit_message>
Fixed excel chart bullshit
</commit_message>
<xml_diff>
--- a/NWSection_2016_Standings.xlsx
+++ b/NWSection_2016_Standings.xlsx
@@ -43,10 +43,10 @@
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{841E416B-1EF1-43b6-AB56-02D37102CBD5}">
       <x15:pivotCaches>
-        <pivotCache cacheId="20" r:id="rId12"/>
-        <pivotCache cacheId="23" r:id="rId13"/>
-        <pivotCache cacheId="41" r:id="rId14"/>
-        <pivotCache cacheId="52" r:id="rId15"/>
+        <pivotCache cacheId="0" r:id="rId12"/>
+        <pivotCache cacheId="1" r:id="rId13"/>
+        <pivotCache cacheId="2" r:id="rId14"/>
+        <pivotCache cacheId="3" r:id="rId15"/>
       </x15:pivotCaches>
     </ext>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{983426D0-5260-488c-9760-48F4B6AC55F4}">
@@ -2203,6 +2203,11 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <colors>
+    <mruColors>
+      <color rgb="FFCDCDCD"/>
+    </mruColors>
+  </colors>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -2330,6 +2335,236 @@
       </c:pivotFmt>
       <c:pivotFmt>
         <c:idx val="10"/>
+        <c:dLbl>
+          <c:idx val="0"/>
+          <c:dLblPos val="ctr"/>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="1"/>
+          <c:showBubbleSize val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
+          </c:extLst>
+        </c:dLbl>
+      </c:pivotFmt>
+      <c:pivotFmt>
+        <c:idx val="11"/>
+        <c:dLbl>
+          <c:idx val="0"/>
+          <c:layout>
+            <c:manualLayout>
+              <c:x val="-9.3999639788354388E-3"/>
+              <c:y val="-3.2009279623121854E-2"/>
+            </c:manualLayout>
+          </c:layout>
+          <c:dLblPos val="bestFit"/>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="1"/>
+          <c:showBubbleSize val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
+          </c:extLst>
+        </c:dLbl>
+      </c:pivotFmt>
+      <c:pivotFmt>
+        <c:idx val="12"/>
+        <c:dLbl>
+          <c:idx val="0"/>
+          <c:layout>
+            <c:manualLayout>
+              <c:x val="1.1491035126308006E-2"/>
+              <c:y val="-2.9577040256178525E-2"/>
+            </c:manualLayout>
+          </c:layout>
+          <c:dLblPos val="bestFit"/>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="1"/>
+          <c:showBubbleSize val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
+          </c:extLst>
+        </c:dLbl>
+      </c:pivotFmt>
+      <c:pivotFmt>
+        <c:idx val="13"/>
+        <c:dLbl>
+          <c:idx val="0"/>
+          <c:layout>
+            <c:manualLayout>
+              <c:x val="-6.254777413311664E-3"/>
+              <c:y val="-2.1826022789029894E-2"/>
+            </c:manualLayout>
+          </c:layout>
+          <c:dLblPos val="bestFit"/>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="1"/>
+          <c:showBubbleSize val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
+          </c:extLst>
+        </c:dLbl>
+      </c:pivotFmt>
+      <c:pivotFmt>
+        <c:idx val="14"/>
+        <c:dLbl>
+          <c:idx val="0"/>
+          <c:layout>
+            <c:manualLayout>
+              <c:x val="-8.5388596039657309E-3"/>
+              <c:y val="-1.5143932838169043E-2"/>
+            </c:manualLayout>
+          </c:layout>
+          <c:dLblPos val="bestFit"/>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="1"/>
+          <c:showBubbleSize val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
+          </c:extLst>
+        </c:dLbl>
+      </c:pivotFmt>
+      <c:pivotFmt>
+        <c:idx val="15"/>
+        <c:dLbl>
+          <c:idx val="0"/>
+          <c:layout>
+            <c:manualLayout>
+              <c:x val="9.2278707379091593E-2"/>
+              <c:y val="6.7995747460030037E-2"/>
+            </c:manualLayout>
+          </c:layout>
+          <c:dLblPos val="bestFit"/>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="1"/>
+          <c:showBubbleSize val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
+          </c:extLst>
+        </c:dLbl>
+      </c:pivotFmt>
+      <c:pivotFmt>
+        <c:idx val="16"/>
+        <c:dLbl>
+          <c:idx val="0"/>
+          <c:layout>
+            <c:manualLayout>
+              <c:x val="0.11476243758340531"/>
+              <c:y val="-5.6022807648696674E-2"/>
+            </c:manualLayout>
+          </c:layout>
+          <c:dLblPos val="bestFit"/>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="1"/>
+          <c:showBubbleSize val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
+          </c:extLst>
+        </c:dLbl>
+      </c:pivotFmt>
+      <c:pivotFmt>
+        <c:idx val="17"/>
+        <c:dLbl>
+          <c:idx val="0"/>
+          <c:layout>
+            <c:manualLayout>
+              <c:x val="-1.4173760992482354E-2"/>
+              <c:y val="-0.17241033328320052"/>
+            </c:manualLayout>
+          </c:layout>
+          <c:dLblPos val="bestFit"/>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="1"/>
+          <c:showBubbleSize val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
+          </c:extLst>
+        </c:dLbl>
+      </c:pivotFmt>
+      <c:pivotFmt>
+        <c:idx val="18"/>
+      </c:pivotFmt>
+      <c:pivotFmt>
+        <c:idx val="19"/>
+      </c:pivotFmt>
+      <c:pivotFmt>
+        <c:idx val="20"/>
+      </c:pivotFmt>
+      <c:pivotFmt>
+        <c:idx val="21"/>
+      </c:pivotFmt>
+      <c:pivotFmt>
+        <c:idx val="22"/>
+      </c:pivotFmt>
+      <c:pivotFmt>
+        <c:idx val="23"/>
+      </c:pivotFmt>
+      <c:pivotFmt>
+        <c:idx val="24"/>
+      </c:pivotFmt>
+      <c:pivotFmt>
+        <c:idx val="25"/>
+      </c:pivotFmt>
+      <c:pivotFmt>
+        <c:idx val="26"/>
+        <c:dLbl>
+          <c:idx val="0"/>
+          <c:showLegendKey val="1"/>
+          <c:showVal val="1"/>
+          <c:showCatName val="1"/>
+          <c:showSerName val="1"/>
+          <c:showPercent val="1"/>
+          <c:showBubbleSize val="1"/>
+          <c:extLst>
+            <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
+          </c:extLst>
+        </c:dLbl>
+      </c:pivotFmt>
+      <c:pivotFmt>
+        <c:idx val="27"/>
+      </c:pivotFmt>
+      <c:pivotFmt>
+        <c:idx val="28"/>
+        <c:spPr>
+          <a:solidFill>
+            <a:schemeClr val="accent1"/>
+          </a:solidFill>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst>
+            <a:outerShdw blurRad="254000" sx="102000" sy="102000" algn="ctr" rotWithShape="0">
+              <a:prstClr val="black">
+                <a:alpha val="20000"/>
+              </a:prstClr>
+            </a:outerShdw>
+          </a:effectLst>
+        </c:spPr>
+      </c:pivotFmt>
+      <c:pivotFmt>
+        <c:idx val="29"/>
         <c:spPr>
           <a:solidFill>
             <a:schemeClr val="accent1"/>
@@ -2353,16 +2588,16 @@
           <c:spPr>
             <a:pattFill prst="pct75">
               <a:fgClr>
-                <a:sysClr val="windowText" lastClr="000000">
+                <a:schemeClr val="dk1">
                   <a:lumMod val="75000"/>
                   <a:lumOff val="25000"/>
-                </a:sysClr>
+                </a:schemeClr>
               </a:fgClr>
               <a:bgClr>
-                <a:sysClr val="windowText" lastClr="000000">
+                <a:schemeClr val="dk1">
                   <a:lumMod val="65000"/>
                   <a:lumOff val="35000"/>
-                </a:sysClr>
+                </a:schemeClr>
               </a:bgClr>
             </a:pattFill>
             <a:ln>
@@ -2395,20 +2630,19 @@
               <a:endParaRPr lang="en-US"/>
             </a:p>
           </c:txPr>
-          <c:dLblPos val="ctr"/>
-          <c:showLegendKey val="0"/>
-          <c:showVal val="0"/>
-          <c:showCatName val="0"/>
-          <c:showSerName val="0"/>
+          <c:showLegendKey val="1"/>
+          <c:showVal val="1"/>
+          <c:showCatName val="1"/>
+          <c:showSerName val="1"/>
           <c:showPercent val="1"/>
-          <c:showBubbleSize val="0"/>
+          <c:showBubbleSize val="1"/>
           <c:extLst>
             <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
           </c:extLst>
         </c:dLbl>
       </c:pivotFmt>
       <c:pivotFmt>
-        <c:idx val="11"/>
+        <c:idx val="30"/>
         <c:spPr>
           <a:solidFill>
             <a:schemeClr val="accent1"/>
@@ -2424,27 +2658,132 @@
             </a:outerShdw>
           </a:effectLst>
         </c:spPr>
+      </c:pivotFmt>
+      <c:pivotFmt>
+        <c:idx val="31"/>
+        <c:spPr>
+          <a:solidFill>
+            <a:schemeClr val="accent1"/>
+          </a:solidFill>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst>
+            <a:outerShdw blurRad="254000" sx="102000" sy="102000" algn="ctr" rotWithShape="0">
+              <a:prstClr val="black">
+                <a:alpha val="20000"/>
+              </a:prstClr>
+            </a:outerShdw>
+          </a:effectLst>
+        </c:spPr>
+      </c:pivotFmt>
+      <c:pivotFmt>
+        <c:idx val="32"/>
+        <c:spPr>
+          <a:solidFill>
+            <a:schemeClr val="accent1"/>
+          </a:solidFill>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst>
+            <a:outerShdw blurRad="254000" sx="102000" sy="102000" algn="ctr" rotWithShape="0">
+              <a:prstClr val="black">
+                <a:alpha val="20000"/>
+              </a:prstClr>
+            </a:outerShdw>
+          </a:effectLst>
+        </c:spPr>
+      </c:pivotFmt>
+      <c:pivotFmt>
+        <c:idx val="33"/>
+        <c:spPr>
+          <a:solidFill>
+            <a:schemeClr val="accent1"/>
+          </a:solidFill>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst>
+            <a:outerShdw blurRad="254000" sx="102000" sy="102000" algn="ctr" rotWithShape="0">
+              <a:prstClr val="black">
+                <a:alpha val="20000"/>
+              </a:prstClr>
+            </a:outerShdw>
+          </a:effectLst>
+        </c:spPr>
+      </c:pivotFmt>
+      <c:pivotFmt>
+        <c:idx val="34"/>
+        <c:spPr>
+          <a:solidFill>
+            <a:schemeClr val="accent1"/>
+          </a:solidFill>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst>
+            <a:outerShdw blurRad="254000" sx="102000" sy="102000" algn="ctr" rotWithShape="0">
+              <a:prstClr val="black">
+                <a:alpha val="20000"/>
+              </a:prstClr>
+            </a:outerShdw>
+          </a:effectLst>
+        </c:spPr>
+      </c:pivotFmt>
+      <c:pivotFmt>
+        <c:idx val="35"/>
+        <c:spPr>
+          <a:solidFill>
+            <a:schemeClr val="accent1"/>
+          </a:solidFill>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst>
+            <a:outerShdw blurRad="254000" sx="102000" sy="102000" algn="ctr" rotWithShape="0">
+              <a:prstClr val="black">
+                <a:alpha val="20000"/>
+              </a:prstClr>
+            </a:outerShdw>
+          </a:effectLst>
+        </c:spPr>
+      </c:pivotFmt>
+      <c:pivotFmt>
+        <c:idx val="36"/>
+        <c:spPr>
+          <a:solidFill>
+            <a:schemeClr val="accent1"/>
+          </a:solidFill>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst>
+            <a:outerShdw blurRad="254000" sx="102000" sy="102000" algn="ctr" rotWithShape="0">
+              <a:prstClr val="black">
+                <a:alpha val="20000"/>
+              </a:prstClr>
+            </a:outerShdw>
+          </a:effectLst>
+        </c:spPr>
+      </c:pivotFmt>
+      <c:pivotFmt>
+        <c:idx val="37"/>
         <c:dLbl>
           <c:idx val="0"/>
-          <c:layout>
-            <c:manualLayout>
-              <c:x val="-9.3999639788354388E-3"/>
-              <c:y val="-3.2009279623121854E-2"/>
-            </c:manualLayout>
-          </c:layout>
           <c:spPr>
             <a:pattFill prst="pct75">
               <a:fgClr>
-                <a:sysClr val="windowText" lastClr="000000">
+                <a:schemeClr val="dk1">
                   <a:lumMod val="75000"/>
                   <a:lumOff val="25000"/>
-                </a:sysClr>
+                </a:schemeClr>
               </a:fgClr>
               <a:bgClr>
-                <a:sysClr val="windowText" lastClr="000000">
+                <a:schemeClr val="dk1">
                   <a:lumMod val="65000"/>
                   <a:lumOff val="35000"/>
-                </a:sysClr>
+                </a:schemeClr>
               </a:bgClr>
             </a:pattFill>
             <a:ln>
@@ -2477,707 +2816,15 @@
               <a:endParaRPr lang="en-US"/>
             </a:p>
           </c:txPr>
-          <c:dLblPos val="bestFit"/>
           <c:showLegendKey val="0"/>
           <c:showVal val="0"/>
           <c:showCatName val="0"/>
           <c:showSerName val="0"/>
           <c:showPercent val="1"/>
-          <c:showBubbleSize val="0"/>
+          <c:showBubbleSize val="1"/>
           <c:extLst>
             <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
           </c:extLst>
-        </c:dLbl>
-      </c:pivotFmt>
-      <c:pivotFmt>
-        <c:idx val="12"/>
-        <c:spPr>
-          <a:solidFill>
-            <a:schemeClr val="accent1"/>
-          </a:solidFill>
-          <a:ln>
-            <a:noFill/>
-          </a:ln>
-          <a:effectLst>
-            <a:outerShdw blurRad="254000" sx="102000" sy="102000" algn="ctr" rotWithShape="0">
-              <a:prstClr val="black">
-                <a:alpha val="20000"/>
-              </a:prstClr>
-            </a:outerShdw>
-          </a:effectLst>
-        </c:spPr>
-        <c:dLbl>
-          <c:idx val="0"/>
-          <c:layout>
-            <c:manualLayout>
-              <c:x val="1.1491035126308006E-2"/>
-              <c:y val="-2.9577040256178525E-2"/>
-            </c:manualLayout>
-          </c:layout>
-          <c:spPr>
-            <a:pattFill prst="pct75">
-              <a:fgClr>
-                <a:sysClr val="windowText" lastClr="000000">
-                  <a:lumMod val="75000"/>
-                  <a:lumOff val="25000"/>
-                </a:sysClr>
-              </a:fgClr>
-              <a:bgClr>
-                <a:sysClr val="windowText" lastClr="000000">
-                  <a:lumMod val="65000"/>
-                  <a:lumOff val="35000"/>
-                </a:sysClr>
-              </a:bgClr>
-            </a:pattFill>
-            <a:ln>
-              <a:noFill/>
-            </a:ln>
-            <a:effectLst>
-              <a:outerShdw blurRad="50800" dist="38100" dir="2700000" algn="tl" rotWithShape="0">
-                <a:prstClr val="black">
-                  <a:alpha val="40000"/>
-                </a:prstClr>
-              </a:outerShdw>
-            </a:effectLst>
-          </c:spPr>
-          <c:txPr>
-            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
-              <a:spAutoFit/>
-            </a:bodyPr>
-            <a:lstStyle/>
-            <a:p>
-              <a:pPr>
-                <a:defRPr sz="1000" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-                  <a:solidFill>
-                    <a:schemeClr val="lt1"/>
-                  </a:solidFill>
-                  <a:latin typeface="+mn-lt"/>
-                  <a:ea typeface="+mn-ea"/>
-                  <a:cs typeface="+mn-cs"/>
-                </a:defRPr>
-              </a:pPr>
-              <a:endParaRPr lang="en-US"/>
-            </a:p>
-          </c:txPr>
-          <c:dLblPos val="bestFit"/>
-          <c:showLegendKey val="0"/>
-          <c:showVal val="0"/>
-          <c:showCatName val="0"/>
-          <c:showSerName val="0"/>
-          <c:showPercent val="1"/>
-          <c:showBubbleSize val="0"/>
-          <c:extLst>
-            <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
-          </c:extLst>
-        </c:dLbl>
-      </c:pivotFmt>
-      <c:pivotFmt>
-        <c:idx val="13"/>
-        <c:spPr>
-          <a:solidFill>
-            <a:schemeClr val="accent1"/>
-          </a:solidFill>
-          <a:ln>
-            <a:noFill/>
-          </a:ln>
-          <a:effectLst>
-            <a:outerShdw blurRad="254000" sx="102000" sy="102000" algn="ctr" rotWithShape="0">
-              <a:prstClr val="black">
-                <a:alpha val="20000"/>
-              </a:prstClr>
-            </a:outerShdw>
-          </a:effectLst>
-        </c:spPr>
-        <c:dLbl>
-          <c:idx val="0"/>
-          <c:layout>
-            <c:manualLayout>
-              <c:x val="-6.254777413311664E-3"/>
-              <c:y val="-2.1826022789029894E-2"/>
-            </c:manualLayout>
-          </c:layout>
-          <c:spPr>
-            <a:pattFill prst="pct75">
-              <a:fgClr>
-                <a:sysClr val="windowText" lastClr="000000">
-                  <a:lumMod val="75000"/>
-                  <a:lumOff val="25000"/>
-                </a:sysClr>
-              </a:fgClr>
-              <a:bgClr>
-                <a:sysClr val="windowText" lastClr="000000">
-                  <a:lumMod val="65000"/>
-                  <a:lumOff val="35000"/>
-                </a:sysClr>
-              </a:bgClr>
-            </a:pattFill>
-            <a:ln>
-              <a:noFill/>
-            </a:ln>
-            <a:effectLst>
-              <a:outerShdw blurRad="50800" dist="38100" dir="2700000" algn="tl" rotWithShape="0">
-                <a:prstClr val="black">
-                  <a:alpha val="40000"/>
-                </a:prstClr>
-              </a:outerShdw>
-            </a:effectLst>
-          </c:spPr>
-          <c:txPr>
-            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
-              <a:spAutoFit/>
-            </a:bodyPr>
-            <a:lstStyle/>
-            <a:p>
-              <a:pPr>
-                <a:defRPr sz="1000" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-                  <a:solidFill>
-                    <a:schemeClr val="lt1"/>
-                  </a:solidFill>
-                  <a:latin typeface="+mn-lt"/>
-                  <a:ea typeface="+mn-ea"/>
-                  <a:cs typeface="+mn-cs"/>
-                </a:defRPr>
-              </a:pPr>
-              <a:endParaRPr lang="en-US"/>
-            </a:p>
-          </c:txPr>
-          <c:dLblPos val="bestFit"/>
-          <c:showLegendKey val="0"/>
-          <c:showVal val="0"/>
-          <c:showCatName val="0"/>
-          <c:showSerName val="0"/>
-          <c:showPercent val="1"/>
-          <c:showBubbleSize val="0"/>
-          <c:extLst>
-            <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
-          </c:extLst>
-        </c:dLbl>
-      </c:pivotFmt>
-      <c:pivotFmt>
-        <c:idx val="14"/>
-        <c:spPr>
-          <a:solidFill>
-            <a:schemeClr val="accent1"/>
-          </a:solidFill>
-          <a:ln>
-            <a:noFill/>
-          </a:ln>
-          <a:effectLst>
-            <a:outerShdw blurRad="254000" sx="102000" sy="102000" algn="ctr" rotWithShape="0">
-              <a:prstClr val="black">
-                <a:alpha val="20000"/>
-              </a:prstClr>
-            </a:outerShdw>
-          </a:effectLst>
-        </c:spPr>
-        <c:dLbl>
-          <c:idx val="0"/>
-          <c:layout>
-            <c:manualLayout>
-              <c:x val="-8.5388596039657309E-3"/>
-              <c:y val="-1.5143932838169043E-2"/>
-            </c:manualLayout>
-          </c:layout>
-          <c:spPr>
-            <a:pattFill prst="pct75">
-              <a:fgClr>
-                <a:sysClr val="windowText" lastClr="000000">
-                  <a:lumMod val="75000"/>
-                  <a:lumOff val="25000"/>
-                </a:sysClr>
-              </a:fgClr>
-              <a:bgClr>
-                <a:sysClr val="windowText" lastClr="000000">
-                  <a:lumMod val="65000"/>
-                  <a:lumOff val="35000"/>
-                </a:sysClr>
-              </a:bgClr>
-            </a:pattFill>
-            <a:ln>
-              <a:noFill/>
-            </a:ln>
-            <a:effectLst>
-              <a:outerShdw blurRad="50800" dist="38100" dir="2700000" algn="tl" rotWithShape="0">
-                <a:prstClr val="black">
-                  <a:alpha val="40000"/>
-                </a:prstClr>
-              </a:outerShdw>
-            </a:effectLst>
-          </c:spPr>
-          <c:txPr>
-            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
-              <a:spAutoFit/>
-            </a:bodyPr>
-            <a:lstStyle/>
-            <a:p>
-              <a:pPr>
-                <a:defRPr sz="1000" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-                  <a:solidFill>
-                    <a:schemeClr val="lt1"/>
-                  </a:solidFill>
-                  <a:latin typeface="+mn-lt"/>
-                  <a:ea typeface="+mn-ea"/>
-                  <a:cs typeface="+mn-cs"/>
-                </a:defRPr>
-              </a:pPr>
-              <a:endParaRPr lang="en-US"/>
-            </a:p>
-          </c:txPr>
-          <c:dLblPos val="bestFit"/>
-          <c:showLegendKey val="0"/>
-          <c:showVal val="0"/>
-          <c:showCatName val="0"/>
-          <c:showSerName val="0"/>
-          <c:showPercent val="1"/>
-          <c:showBubbleSize val="0"/>
-          <c:extLst>
-            <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
-          </c:extLst>
-        </c:dLbl>
-      </c:pivotFmt>
-      <c:pivotFmt>
-        <c:idx val="15"/>
-        <c:spPr>
-          <a:solidFill>
-            <a:schemeClr val="accent1"/>
-          </a:solidFill>
-          <a:ln>
-            <a:noFill/>
-          </a:ln>
-          <a:effectLst>
-            <a:outerShdw blurRad="254000" sx="102000" sy="102000" algn="ctr" rotWithShape="0">
-              <a:prstClr val="black">
-                <a:alpha val="20000"/>
-              </a:prstClr>
-            </a:outerShdw>
-          </a:effectLst>
-        </c:spPr>
-        <c:dLbl>
-          <c:idx val="0"/>
-          <c:layout>
-            <c:manualLayout>
-              <c:x val="9.2278707379091593E-2"/>
-              <c:y val="6.7995747460030037E-2"/>
-            </c:manualLayout>
-          </c:layout>
-          <c:spPr>
-            <a:pattFill prst="pct75">
-              <a:fgClr>
-                <a:sysClr val="windowText" lastClr="000000">
-                  <a:lumMod val="75000"/>
-                  <a:lumOff val="25000"/>
-                </a:sysClr>
-              </a:fgClr>
-              <a:bgClr>
-                <a:sysClr val="windowText" lastClr="000000">
-                  <a:lumMod val="65000"/>
-                  <a:lumOff val="35000"/>
-                </a:sysClr>
-              </a:bgClr>
-            </a:pattFill>
-            <a:ln>
-              <a:noFill/>
-            </a:ln>
-            <a:effectLst>
-              <a:outerShdw blurRad="50800" dist="38100" dir="2700000" algn="tl" rotWithShape="0">
-                <a:prstClr val="black">
-                  <a:alpha val="40000"/>
-                </a:prstClr>
-              </a:outerShdw>
-            </a:effectLst>
-          </c:spPr>
-          <c:txPr>
-            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
-              <a:spAutoFit/>
-            </a:bodyPr>
-            <a:lstStyle/>
-            <a:p>
-              <a:pPr>
-                <a:defRPr sz="1000" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-                  <a:solidFill>
-                    <a:schemeClr val="lt1"/>
-                  </a:solidFill>
-                  <a:latin typeface="+mn-lt"/>
-                  <a:ea typeface="+mn-ea"/>
-                  <a:cs typeface="+mn-cs"/>
-                </a:defRPr>
-              </a:pPr>
-              <a:endParaRPr lang="en-US"/>
-            </a:p>
-          </c:txPr>
-          <c:dLblPos val="bestFit"/>
-          <c:showLegendKey val="0"/>
-          <c:showVal val="0"/>
-          <c:showCatName val="0"/>
-          <c:showSerName val="0"/>
-          <c:showPercent val="1"/>
-          <c:showBubbleSize val="0"/>
-          <c:extLst>
-            <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
-          </c:extLst>
-        </c:dLbl>
-      </c:pivotFmt>
-      <c:pivotFmt>
-        <c:idx val="16"/>
-        <c:spPr>
-          <a:solidFill>
-            <a:schemeClr val="accent1"/>
-          </a:solidFill>
-          <a:ln>
-            <a:noFill/>
-          </a:ln>
-          <a:effectLst>
-            <a:outerShdw blurRad="254000" sx="102000" sy="102000" algn="ctr" rotWithShape="0">
-              <a:prstClr val="black">
-                <a:alpha val="20000"/>
-              </a:prstClr>
-            </a:outerShdw>
-          </a:effectLst>
-        </c:spPr>
-        <c:dLbl>
-          <c:idx val="0"/>
-          <c:layout>
-            <c:manualLayout>
-              <c:x val="0.11476243758340531"/>
-              <c:y val="-5.6022807648696674E-2"/>
-            </c:manualLayout>
-          </c:layout>
-          <c:spPr>
-            <a:pattFill prst="pct75">
-              <a:fgClr>
-                <a:sysClr val="windowText" lastClr="000000">
-                  <a:lumMod val="75000"/>
-                  <a:lumOff val="25000"/>
-                </a:sysClr>
-              </a:fgClr>
-              <a:bgClr>
-                <a:sysClr val="windowText" lastClr="000000">
-                  <a:lumMod val="65000"/>
-                  <a:lumOff val="35000"/>
-                </a:sysClr>
-              </a:bgClr>
-            </a:pattFill>
-            <a:ln>
-              <a:noFill/>
-            </a:ln>
-            <a:effectLst>
-              <a:outerShdw blurRad="50800" dist="38100" dir="2700000" algn="tl" rotWithShape="0">
-                <a:prstClr val="black">
-                  <a:alpha val="40000"/>
-                </a:prstClr>
-              </a:outerShdw>
-            </a:effectLst>
-          </c:spPr>
-          <c:txPr>
-            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
-              <a:spAutoFit/>
-            </a:bodyPr>
-            <a:lstStyle/>
-            <a:p>
-              <a:pPr>
-                <a:defRPr sz="1000" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-                  <a:solidFill>
-                    <a:schemeClr val="lt1"/>
-                  </a:solidFill>
-                  <a:latin typeface="+mn-lt"/>
-                  <a:ea typeface="+mn-ea"/>
-                  <a:cs typeface="+mn-cs"/>
-                </a:defRPr>
-              </a:pPr>
-              <a:endParaRPr lang="en-US"/>
-            </a:p>
-          </c:txPr>
-          <c:dLblPos val="bestFit"/>
-          <c:showLegendKey val="0"/>
-          <c:showVal val="0"/>
-          <c:showCatName val="0"/>
-          <c:showSerName val="0"/>
-          <c:showPercent val="1"/>
-          <c:showBubbleSize val="0"/>
-          <c:extLst>
-            <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
-          </c:extLst>
-        </c:dLbl>
-      </c:pivotFmt>
-      <c:pivotFmt>
-        <c:idx val="17"/>
-        <c:spPr>
-          <a:solidFill>
-            <a:schemeClr val="accent1"/>
-          </a:solidFill>
-          <a:ln>
-            <a:noFill/>
-          </a:ln>
-          <a:effectLst>
-            <a:outerShdw blurRad="254000" sx="102000" sy="102000" algn="ctr" rotWithShape="0">
-              <a:prstClr val="black">
-                <a:alpha val="20000"/>
-              </a:prstClr>
-            </a:outerShdw>
-          </a:effectLst>
-        </c:spPr>
-        <c:dLbl>
-          <c:idx val="0"/>
-          <c:layout>
-            <c:manualLayout>
-              <c:x val="-1.4173760992482354E-2"/>
-              <c:y val="-0.17241033328320052"/>
-            </c:manualLayout>
-          </c:layout>
-          <c:spPr>
-            <a:pattFill prst="pct75">
-              <a:fgClr>
-                <a:sysClr val="windowText" lastClr="000000">
-                  <a:lumMod val="75000"/>
-                  <a:lumOff val="25000"/>
-                </a:sysClr>
-              </a:fgClr>
-              <a:bgClr>
-                <a:sysClr val="windowText" lastClr="000000">
-                  <a:lumMod val="65000"/>
-                  <a:lumOff val="35000"/>
-                </a:sysClr>
-              </a:bgClr>
-            </a:pattFill>
-            <a:ln>
-              <a:noFill/>
-            </a:ln>
-            <a:effectLst>
-              <a:outerShdw blurRad="50800" dist="38100" dir="2700000" algn="tl" rotWithShape="0">
-                <a:prstClr val="black">
-                  <a:alpha val="40000"/>
-                </a:prstClr>
-              </a:outerShdw>
-            </a:effectLst>
-          </c:spPr>
-          <c:txPr>
-            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
-              <a:spAutoFit/>
-            </a:bodyPr>
-            <a:lstStyle/>
-            <a:p>
-              <a:pPr>
-                <a:defRPr sz="1000" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-                  <a:solidFill>
-                    <a:schemeClr val="lt1"/>
-                  </a:solidFill>
-                  <a:latin typeface="+mn-lt"/>
-                  <a:ea typeface="+mn-ea"/>
-                  <a:cs typeface="+mn-cs"/>
-                </a:defRPr>
-              </a:pPr>
-              <a:endParaRPr lang="en-US"/>
-            </a:p>
-          </c:txPr>
-          <c:dLblPos val="bestFit"/>
-          <c:showLegendKey val="0"/>
-          <c:showVal val="0"/>
-          <c:showCatName val="0"/>
-          <c:showSerName val="0"/>
-          <c:showPercent val="1"/>
-          <c:showBubbleSize val="0"/>
-          <c:extLst>
-            <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
-          </c:extLst>
-        </c:dLbl>
-      </c:pivotFmt>
-      <c:pivotFmt>
-        <c:idx val="18"/>
-        <c:spPr>
-          <a:solidFill>
-            <a:schemeClr val="accent1"/>
-          </a:solidFill>
-          <a:ln>
-            <a:noFill/>
-          </a:ln>
-          <a:effectLst>
-            <a:outerShdw blurRad="254000" sx="102000" sy="102000" algn="ctr" rotWithShape="0">
-              <a:prstClr val="black">
-                <a:alpha val="20000"/>
-              </a:prstClr>
-            </a:outerShdw>
-          </a:effectLst>
-        </c:spPr>
-      </c:pivotFmt>
-      <c:pivotFmt>
-        <c:idx val="19"/>
-        <c:spPr>
-          <a:solidFill>
-            <a:schemeClr val="accent2"/>
-          </a:solidFill>
-          <a:ln>
-            <a:noFill/>
-          </a:ln>
-          <a:effectLst>
-            <a:outerShdw blurRad="254000" sx="102000" sy="102000" algn="ctr" rotWithShape="0">
-              <a:prstClr val="black">
-                <a:alpha val="20000"/>
-              </a:prstClr>
-            </a:outerShdw>
-          </a:effectLst>
-        </c:spPr>
-      </c:pivotFmt>
-      <c:pivotFmt>
-        <c:idx val="20"/>
-        <c:spPr>
-          <a:solidFill>
-            <a:schemeClr val="accent3"/>
-          </a:solidFill>
-          <a:ln>
-            <a:noFill/>
-          </a:ln>
-          <a:effectLst>
-            <a:outerShdw blurRad="254000" sx="102000" sy="102000" algn="ctr" rotWithShape="0">
-              <a:prstClr val="black">
-                <a:alpha val="20000"/>
-              </a:prstClr>
-            </a:outerShdw>
-          </a:effectLst>
-        </c:spPr>
-      </c:pivotFmt>
-      <c:pivotFmt>
-        <c:idx val="21"/>
-        <c:spPr>
-          <a:solidFill>
-            <a:schemeClr val="accent4"/>
-          </a:solidFill>
-          <a:ln>
-            <a:noFill/>
-          </a:ln>
-          <a:effectLst>
-            <a:outerShdw blurRad="254000" sx="102000" sy="102000" algn="ctr" rotWithShape="0">
-              <a:prstClr val="black">
-                <a:alpha val="20000"/>
-              </a:prstClr>
-            </a:outerShdw>
-          </a:effectLst>
-        </c:spPr>
-      </c:pivotFmt>
-      <c:pivotFmt>
-        <c:idx val="22"/>
-        <c:spPr>
-          <a:solidFill>
-            <a:schemeClr val="accent5"/>
-          </a:solidFill>
-          <a:ln>
-            <a:noFill/>
-          </a:ln>
-          <a:effectLst>
-            <a:outerShdw blurRad="254000" sx="102000" sy="102000" algn="ctr" rotWithShape="0">
-              <a:prstClr val="black">
-                <a:alpha val="20000"/>
-              </a:prstClr>
-            </a:outerShdw>
-          </a:effectLst>
-        </c:spPr>
-      </c:pivotFmt>
-      <c:pivotFmt>
-        <c:idx val="23"/>
-        <c:spPr>
-          <a:solidFill>
-            <a:schemeClr val="accent6"/>
-          </a:solidFill>
-          <a:ln>
-            <a:noFill/>
-          </a:ln>
-          <a:effectLst>
-            <a:outerShdw blurRad="254000" sx="102000" sy="102000" algn="ctr" rotWithShape="0">
-              <a:prstClr val="black">
-                <a:alpha val="20000"/>
-              </a:prstClr>
-            </a:outerShdw>
-          </a:effectLst>
-        </c:spPr>
-      </c:pivotFmt>
-      <c:pivotFmt>
-        <c:idx val="24"/>
-        <c:spPr>
-          <a:solidFill>
-            <a:schemeClr val="accent1">
-              <a:lumMod val="60000"/>
-            </a:schemeClr>
-          </a:solidFill>
-          <a:ln>
-            <a:noFill/>
-          </a:ln>
-          <a:effectLst>
-            <a:outerShdw blurRad="254000" sx="102000" sy="102000" algn="ctr" rotWithShape="0">
-              <a:prstClr val="black">
-                <a:alpha val="20000"/>
-              </a:prstClr>
-            </a:outerShdw>
-          </a:effectLst>
-        </c:spPr>
-      </c:pivotFmt>
-      <c:pivotFmt>
-        <c:idx val="25"/>
-        <c:spPr>
-          <a:solidFill>
-            <a:schemeClr val="accent2">
-              <a:lumMod val="60000"/>
-            </a:schemeClr>
-          </a:solidFill>
-          <a:ln>
-            <a:noFill/>
-          </a:ln>
-          <a:effectLst>
-            <a:outerShdw blurRad="254000" sx="102000" sy="102000" algn="ctr" rotWithShape="0">
-              <a:prstClr val="black">
-                <a:alpha val="20000"/>
-              </a:prstClr>
-            </a:outerShdw>
-          </a:effectLst>
-        </c:spPr>
-      </c:pivotFmt>
-      <c:pivotFmt>
-        <c:idx val="26"/>
-        <c:dLbl>
-          <c:idx val="0"/>
-          <c:spPr>
-            <a:pattFill prst="pct75">
-              <a:fgClr>
-                <a:sysClr val="windowText" lastClr="000000">
-                  <a:lumMod val="75000"/>
-                  <a:lumOff val="25000"/>
-                </a:sysClr>
-              </a:fgClr>
-              <a:bgClr>
-                <a:sysClr val="windowText" lastClr="000000">
-                  <a:lumMod val="65000"/>
-                  <a:lumOff val="35000"/>
-                </a:sysClr>
-              </a:bgClr>
-            </a:pattFill>
-            <a:ln>
-              <a:noFill/>
-            </a:ln>
-            <a:effectLst>
-              <a:outerShdw blurRad="50800" dist="38100" dir="2700000" algn="tl" rotWithShape="0">
-                <a:prstClr val="black">
-                  <a:alpha val="40000"/>
-                </a:prstClr>
-              </a:outerShdw>
-            </a:effectLst>
-          </c:spPr>
-          <c:txPr>
-            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
-              <a:spAutoFit/>
-            </a:bodyPr>
-            <a:lstStyle/>
-            <a:p>
-              <a:pPr>
-                <a:defRPr sz="1600" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-                  <a:solidFill>
-                    <a:schemeClr val="lt1"/>
-                  </a:solidFill>
-                  <a:latin typeface="+mn-lt"/>
-                  <a:ea typeface="+mn-ea"/>
-                  <a:cs typeface="+mn-cs"/>
-                </a:defRPr>
-              </a:pPr>
-              <a:endParaRPr lang="en-US"/>
-            </a:p>
-          </c:txPr>
         </c:dLbl>
       </c:pivotFmt>
     </c:pivotFmts>
@@ -3398,173 +3045,19 @@
             </c:extLst>
           </c:dPt>
           <c:dLbls>
-            <c:dLbl>
-              <c:idx val="1"/>
-              <c:layout>
-                <c:manualLayout>
-                  <c:x val="-1.4173760992482354E-2"/>
-                  <c:y val="-0.17241033328320052"/>
-                </c:manualLayout>
-              </c:layout>
-              <c:dLblPos val="bestFit"/>
-              <c:showLegendKey val="0"/>
-              <c:showVal val="0"/>
-              <c:showCatName val="0"/>
-              <c:showSerName val="0"/>
-              <c:showPercent val="1"/>
-              <c:showBubbleSize val="0"/>
-              <c:extLst>
-                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
-                <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-                  <c16:uniqueId val="{00000008-4573-4DF3-A96E-6617C26101C4}"/>
-                </c:ext>
-              </c:extLst>
-            </c:dLbl>
-            <c:dLbl>
-              <c:idx val="2"/>
-              <c:layout>
-                <c:manualLayout>
-                  <c:x val="0.11476243758340531"/>
-                  <c:y val="-5.6022807648696674E-2"/>
-                </c:manualLayout>
-              </c:layout>
-              <c:dLblPos val="bestFit"/>
-              <c:showLegendKey val="0"/>
-              <c:showVal val="0"/>
-              <c:showCatName val="0"/>
-              <c:showSerName val="0"/>
-              <c:showPercent val="1"/>
-              <c:showBubbleSize val="0"/>
-              <c:extLst>
-                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
-                <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-                  <c16:uniqueId val="{00000007-4573-4DF3-A96E-6617C26101C4}"/>
-                </c:ext>
-              </c:extLst>
-            </c:dLbl>
-            <c:dLbl>
-              <c:idx val="3"/>
-              <c:layout>
-                <c:manualLayout>
-                  <c:x val="9.2278707379091593E-2"/>
-                  <c:y val="6.7995747460030037E-2"/>
-                </c:manualLayout>
-              </c:layout>
-              <c:dLblPos val="bestFit"/>
-              <c:showLegendKey val="0"/>
-              <c:showVal val="0"/>
-              <c:showCatName val="0"/>
-              <c:showSerName val="0"/>
-              <c:showPercent val="1"/>
-              <c:showBubbleSize val="0"/>
-              <c:extLst>
-                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
-                <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-                  <c16:uniqueId val="{00000001-4573-4DF3-A96E-6617C26101C4}"/>
-                </c:ext>
-              </c:extLst>
-            </c:dLbl>
-            <c:dLbl>
-              <c:idx val="4"/>
-              <c:layout>
-                <c:manualLayout>
-                  <c:x val="-8.5388596039657309E-3"/>
-                  <c:y val="-1.5143932838169043E-2"/>
-                </c:manualLayout>
-              </c:layout>
-              <c:dLblPos val="bestFit"/>
-              <c:showLegendKey val="0"/>
-              <c:showVal val="0"/>
-              <c:showCatName val="0"/>
-              <c:showSerName val="0"/>
-              <c:showPercent val="1"/>
-              <c:showBubbleSize val="0"/>
-              <c:extLst>
-                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
-                <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-                  <c16:uniqueId val="{00000002-4573-4DF3-A96E-6617C26101C4}"/>
-                </c:ext>
-              </c:extLst>
-            </c:dLbl>
-            <c:dLbl>
-              <c:idx val="5"/>
-              <c:layout>
-                <c:manualLayout>
-                  <c:x val="-6.254777413311664E-3"/>
-                  <c:y val="-2.1826022789029894E-2"/>
-                </c:manualLayout>
-              </c:layout>
-              <c:dLblPos val="bestFit"/>
-              <c:showLegendKey val="0"/>
-              <c:showVal val="0"/>
-              <c:showCatName val="0"/>
-              <c:showSerName val="0"/>
-              <c:showPercent val="1"/>
-              <c:showBubbleSize val="0"/>
-              <c:extLst>
-                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
-                <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-                  <c16:uniqueId val="{00000003-4573-4DF3-A96E-6617C26101C4}"/>
-                </c:ext>
-              </c:extLst>
-            </c:dLbl>
-            <c:dLbl>
-              <c:idx val="6"/>
-              <c:layout>
-                <c:manualLayout>
-                  <c:x val="-9.3999639788354388E-3"/>
-                  <c:y val="-3.2009279623121854E-2"/>
-                </c:manualLayout>
-              </c:layout>
-              <c:dLblPos val="bestFit"/>
-              <c:showLegendKey val="0"/>
-              <c:showVal val="0"/>
-              <c:showCatName val="0"/>
-              <c:showSerName val="0"/>
-              <c:showPercent val="1"/>
-              <c:showBubbleSize val="0"/>
-              <c:extLst>
-                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
-                <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-                  <c16:uniqueId val="{00000004-4573-4DF3-A96E-6617C26101C4}"/>
-                </c:ext>
-              </c:extLst>
-            </c:dLbl>
-            <c:dLbl>
-              <c:idx val="7"/>
-              <c:layout>
-                <c:manualLayout>
-                  <c:x val="1.1491035126308006E-2"/>
-                  <c:y val="-2.9577040256178525E-2"/>
-                </c:manualLayout>
-              </c:layout>
-              <c:dLblPos val="bestFit"/>
-              <c:showLegendKey val="0"/>
-              <c:showVal val="0"/>
-              <c:showCatName val="0"/>
-              <c:showSerName val="0"/>
-              <c:showPercent val="1"/>
-              <c:showBubbleSize val="0"/>
-              <c:extLst>
-                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
-                <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-                  <c16:uniqueId val="{00000006-4573-4DF3-A96E-6617C26101C4}"/>
-                </c:ext>
-              </c:extLst>
-            </c:dLbl>
             <c:spPr>
               <a:pattFill prst="pct75">
                 <a:fgClr>
-                  <a:sysClr val="windowText" lastClr="000000">
+                  <a:schemeClr val="dk1">
                     <a:lumMod val="75000"/>
                     <a:lumOff val="25000"/>
-                  </a:sysClr>
+                  </a:schemeClr>
                 </a:fgClr>
                 <a:bgClr>
-                  <a:sysClr val="windowText" lastClr="000000">
+                  <a:schemeClr val="dk1">
                     <a:lumMod val="65000"/>
                     <a:lumOff val="35000"/>
-                  </a:sysClr>
+                  </a:schemeClr>
                 </a:bgClr>
               </a:pattFill>
               <a:ln>
@@ -3585,7 +3078,7 @@
               <a:lstStyle/>
               <a:p>
                 <a:pPr>
-                  <a:defRPr sz="1600" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:defRPr sz="1000" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                     <a:solidFill>
                       <a:schemeClr val="lt1"/>
                     </a:solidFill>
@@ -3597,13 +3090,12 @@
                 <a:endParaRPr lang="en-US"/>
               </a:p>
             </c:txPr>
-            <c:dLblPos val="ctr"/>
             <c:showLegendKey val="0"/>
             <c:showVal val="0"/>
             <c:showCatName val="0"/>
             <c:showSerName val="0"/>
             <c:showPercent val="1"/>
-            <c:showBubbleSize val="0"/>
+            <c:showBubbleSize val="1"/>
             <c:showLeaderLines val="1"/>
             <c:leaderLines>
               <c:spPr>
@@ -3690,10 +3182,10 @@
         <c:dLbls>
           <c:dLblPos val="ctr"/>
           <c:showLegendKey val="0"/>
-          <c:showVal val="0"/>
+          <c:showVal val="1"/>
           <c:showCatName val="0"/>
           <c:showSerName val="0"/>
-          <c:showPercent val="1"/>
+          <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
           <c:showLeaderLines val="1"/>
         </c:dLbls>
@@ -6740,13 +6232,8 @@
             </a:pPr>
             <a:r>
               <a:rPr lang="en-US"/>
-              <a:t>Section</a:t>
+              <a:t>Section Member vs Non-Member Participation</a:t>
             </a:r>
-            <a:r>
-              <a:rPr lang="en-US" baseline="0"/>
-              <a:t> Member vs Non-Member Participation</a:t>
-            </a:r>
-            <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:rich>
       </c:tx>
@@ -6786,35 +6273,6 @@
       </c:pivotFmt>
       <c:pivotFmt>
         <c:idx val="1"/>
-        <c:spPr>
-          <a:solidFill>
-            <a:schemeClr val="accent1">
-              <a:alpha val="85000"/>
-            </a:schemeClr>
-          </a:solidFill>
-          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-            <a:solidFill>
-              <a:schemeClr val="lt1">
-                <a:alpha val="50000"/>
-              </a:schemeClr>
-            </a:solidFill>
-            <a:round/>
-          </a:ln>
-          <a:effectLst/>
-        </c:spPr>
-        <c:marker>
-          <c:spPr>
-            <a:solidFill>
-              <a:schemeClr val="accent1">
-                <a:alpha val="85000"/>
-              </a:schemeClr>
-            </a:solidFill>
-            <a:ln>
-              <a:noFill/>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
-        </c:marker>
         <c:dLbl>
           <c:idx val="0"/>
           <c:dLblPos val="inEnd"/>
@@ -6831,35 +6289,6 @@
       </c:pivotFmt>
       <c:pivotFmt>
         <c:idx val="2"/>
-        <c:spPr>
-          <a:solidFill>
-            <a:schemeClr val="accent1">
-              <a:alpha val="85000"/>
-            </a:schemeClr>
-          </a:solidFill>
-          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-            <a:solidFill>
-              <a:schemeClr val="lt1">
-                <a:alpha val="50000"/>
-              </a:schemeClr>
-            </a:solidFill>
-            <a:round/>
-          </a:ln>
-          <a:effectLst/>
-        </c:spPr>
-        <c:marker>
-          <c:spPr>
-            <a:solidFill>
-              <a:schemeClr val="accent1">
-                <a:alpha val="85000"/>
-              </a:schemeClr>
-            </a:solidFill>
-            <a:ln>
-              <a:noFill/>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
-        </c:marker>
         <c:dLbl>
           <c:idx val="0"/>
           <c:dLblPos val="inEnd"/>
@@ -6876,6 +6305,114 @@
       </c:pivotFmt>
       <c:pivotFmt>
         <c:idx val="3"/>
+        <c:dLbl>
+          <c:idx val="0"/>
+          <c:dLblPos val="inEnd"/>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="1"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
+          </c:extLst>
+        </c:dLbl>
+      </c:pivotFmt>
+      <c:pivotFmt>
+        <c:idx val="4"/>
+        <c:dLbl>
+          <c:idx val="0"/>
+          <c:dLblPos val="inEnd"/>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="1"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
+          </c:extLst>
+        </c:dLbl>
+      </c:pivotFmt>
+      <c:pivotFmt>
+        <c:idx val="5"/>
+        <c:dLbl>
+          <c:idx val="0"/>
+          <c:dLblPos val="inEnd"/>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="1"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
+          </c:extLst>
+        </c:dLbl>
+      </c:pivotFmt>
+      <c:pivotFmt>
+        <c:idx val="6"/>
+        <c:dLbl>
+          <c:idx val="0"/>
+          <c:dLblPos val="inEnd"/>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="1"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
+          </c:extLst>
+        </c:dLbl>
+      </c:pivotFmt>
+      <c:pivotFmt>
+        <c:idx val="7"/>
+      </c:pivotFmt>
+      <c:pivotFmt>
+        <c:idx val="8"/>
+        <c:dLbl>
+          <c:idx val="0"/>
+          <c:dLblPos val="inEnd"/>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="1"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
+          </c:extLst>
+        </c:dLbl>
+      </c:pivotFmt>
+      <c:pivotFmt>
+        <c:idx val="9"/>
+        <c:dLbl>
+          <c:idx val="0"/>
+          <c:dLblPos val="inEnd"/>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="1"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
+          </c:extLst>
+        </c:dLbl>
+      </c:pivotFmt>
+      <c:pivotFmt>
+        <c:idx val="10"/>
+      </c:pivotFmt>
+      <c:pivotFmt>
+        <c:idx val="11"/>
+      </c:pivotFmt>
+      <c:pivotFmt>
+        <c:idx val="12"/>
+      </c:pivotFmt>
+      <c:pivotFmt>
+        <c:idx val="13"/>
         <c:spPr>
           <a:solidFill>
             <a:schemeClr val="accent1">
@@ -6911,7 +6448,7 @@
             <a:lstStyle/>
             <a:p>
               <a:pPr>
-                <a:defRPr sz="900" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:defRPr sz="1800" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                   <a:solidFill>
                     <a:schemeClr val="lt1"/>
                   </a:solidFill>
@@ -6936,7 +6473,7 @@
         </c:dLbl>
       </c:pivotFmt>
       <c:pivotFmt>
-        <c:idx val="4"/>
+        <c:idx val="14"/>
         <c:spPr>
           <a:solidFill>
             <a:schemeClr val="accent1">
@@ -6972,7 +6509,7 @@
             <a:lstStyle/>
             <a:p>
               <a:pPr>
-                <a:defRPr sz="900" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:defRPr sz="1800" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                   <a:solidFill>
                     <a:schemeClr val="lt1"/>
                   </a:solidFill>
@@ -6994,387 +6531,6 @@
           <c:extLst>
             <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
           </c:extLst>
-        </c:dLbl>
-      </c:pivotFmt>
-      <c:pivotFmt>
-        <c:idx val="5"/>
-        <c:spPr>
-          <a:solidFill>
-            <a:schemeClr val="accent1">
-              <a:alpha val="85000"/>
-            </a:schemeClr>
-          </a:solidFill>
-          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-            <a:solidFill>
-              <a:schemeClr val="lt1">
-                <a:alpha val="50000"/>
-              </a:schemeClr>
-            </a:solidFill>
-            <a:round/>
-          </a:ln>
-          <a:effectLst/>
-        </c:spPr>
-        <c:marker>
-          <c:symbol val="none"/>
-        </c:marker>
-        <c:dLbl>
-          <c:idx val="0"/>
-          <c:spPr>
-            <a:noFill/>
-            <a:ln>
-              <a:noFill/>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
-          <c:txPr>
-            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
-              <a:spAutoFit/>
-            </a:bodyPr>
-            <a:lstStyle/>
-            <a:p>
-              <a:pPr>
-                <a:defRPr sz="900" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-                  <a:solidFill>
-                    <a:schemeClr val="lt1"/>
-                  </a:solidFill>
-                  <a:latin typeface="+mn-lt"/>
-                  <a:ea typeface="+mn-ea"/>
-                  <a:cs typeface="+mn-cs"/>
-                </a:defRPr>
-              </a:pPr>
-              <a:endParaRPr lang="en-US"/>
-            </a:p>
-          </c:txPr>
-          <c:dLblPos val="inEnd"/>
-          <c:showLegendKey val="0"/>
-          <c:showVal val="1"/>
-          <c:showCatName val="0"/>
-          <c:showSerName val="0"/>
-          <c:showPercent val="0"/>
-          <c:showBubbleSize val="0"/>
-          <c:extLst>
-            <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
-          </c:extLst>
-        </c:dLbl>
-      </c:pivotFmt>
-      <c:pivotFmt>
-        <c:idx val="6"/>
-        <c:spPr>
-          <a:solidFill>
-            <a:schemeClr val="accent1">
-              <a:alpha val="85000"/>
-            </a:schemeClr>
-          </a:solidFill>
-          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-            <a:solidFill>
-              <a:schemeClr val="lt1">
-                <a:alpha val="50000"/>
-              </a:schemeClr>
-            </a:solidFill>
-            <a:round/>
-          </a:ln>
-          <a:effectLst/>
-        </c:spPr>
-        <c:marker>
-          <c:symbol val="none"/>
-        </c:marker>
-        <c:dLbl>
-          <c:idx val="0"/>
-          <c:spPr>
-            <a:noFill/>
-            <a:ln>
-              <a:noFill/>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
-          <c:txPr>
-            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
-              <a:spAutoFit/>
-            </a:bodyPr>
-            <a:lstStyle/>
-            <a:p>
-              <a:pPr>
-                <a:defRPr sz="900" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-                  <a:solidFill>
-                    <a:schemeClr val="lt1"/>
-                  </a:solidFill>
-                  <a:latin typeface="+mn-lt"/>
-                  <a:ea typeface="+mn-ea"/>
-                  <a:cs typeface="+mn-cs"/>
-                </a:defRPr>
-              </a:pPr>
-              <a:endParaRPr lang="en-US"/>
-            </a:p>
-          </c:txPr>
-          <c:dLblPos val="inEnd"/>
-          <c:showLegendKey val="0"/>
-          <c:showVal val="1"/>
-          <c:showCatName val="0"/>
-          <c:showSerName val="0"/>
-          <c:showPercent val="0"/>
-          <c:showBubbleSize val="0"/>
-          <c:extLst>
-            <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
-          </c:extLst>
-        </c:dLbl>
-      </c:pivotFmt>
-      <c:pivotFmt>
-        <c:idx val="7"/>
-        <c:spPr>
-          <a:solidFill>
-            <a:schemeClr val="accent1">
-              <a:alpha val="85000"/>
-            </a:schemeClr>
-          </a:solidFill>
-          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-            <a:solidFill>
-              <a:schemeClr val="lt1">
-                <a:alpha val="50000"/>
-              </a:schemeClr>
-            </a:solidFill>
-            <a:round/>
-          </a:ln>
-          <a:effectLst/>
-        </c:spPr>
-        <c:marker>
-          <c:symbol val="none"/>
-        </c:marker>
-      </c:pivotFmt>
-      <c:pivotFmt>
-        <c:idx val="8"/>
-        <c:spPr>
-          <a:solidFill>
-            <a:schemeClr val="accent1">
-              <a:alpha val="85000"/>
-            </a:schemeClr>
-          </a:solidFill>
-          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-            <a:solidFill>
-              <a:schemeClr val="lt1">
-                <a:alpha val="50000"/>
-              </a:schemeClr>
-            </a:solidFill>
-            <a:round/>
-          </a:ln>
-          <a:effectLst/>
-        </c:spPr>
-        <c:marker>
-          <c:symbol val="none"/>
-        </c:marker>
-        <c:dLbl>
-          <c:idx val="0"/>
-          <c:spPr>
-            <a:noFill/>
-            <a:ln>
-              <a:noFill/>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
-          <c:txPr>
-            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
-              <a:spAutoFit/>
-            </a:bodyPr>
-            <a:lstStyle/>
-            <a:p>
-              <a:pPr>
-                <a:defRPr sz="900" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-                  <a:solidFill>
-                    <a:schemeClr val="lt1"/>
-                  </a:solidFill>
-                  <a:latin typeface="+mn-lt"/>
-                  <a:ea typeface="+mn-ea"/>
-                  <a:cs typeface="+mn-cs"/>
-                </a:defRPr>
-              </a:pPr>
-              <a:endParaRPr lang="en-US"/>
-            </a:p>
-          </c:txPr>
-          <c:dLblPos val="inEnd"/>
-          <c:showLegendKey val="0"/>
-          <c:showVal val="1"/>
-          <c:showCatName val="0"/>
-          <c:showSerName val="0"/>
-          <c:showPercent val="0"/>
-          <c:showBubbleSize val="0"/>
-          <c:extLst>
-            <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
-          </c:extLst>
-        </c:dLbl>
-      </c:pivotFmt>
-      <c:pivotFmt>
-        <c:idx val="9"/>
-        <c:spPr>
-          <a:solidFill>
-            <a:schemeClr val="accent1">
-              <a:alpha val="85000"/>
-            </a:schemeClr>
-          </a:solidFill>
-          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-            <a:solidFill>
-              <a:schemeClr val="lt1">
-                <a:alpha val="50000"/>
-              </a:schemeClr>
-            </a:solidFill>
-            <a:round/>
-          </a:ln>
-          <a:effectLst/>
-        </c:spPr>
-        <c:marker>
-          <c:symbol val="none"/>
-        </c:marker>
-        <c:dLbl>
-          <c:idx val="0"/>
-          <c:spPr>
-            <a:noFill/>
-            <a:ln>
-              <a:noFill/>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
-          <c:txPr>
-            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
-              <a:spAutoFit/>
-            </a:bodyPr>
-            <a:lstStyle/>
-            <a:p>
-              <a:pPr>
-                <a:defRPr sz="900" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-                  <a:solidFill>
-                    <a:schemeClr val="lt1"/>
-                  </a:solidFill>
-                  <a:latin typeface="+mn-lt"/>
-                  <a:ea typeface="+mn-ea"/>
-                  <a:cs typeface="+mn-cs"/>
-                </a:defRPr>
-              </a:pPr>
-              <a:endParaRPr lang="en-US"/>
-            </a:p>
-          </c:txPr>
-          <c:dLblPos val="inEnd"/>
-          <c:showLegendKey val="0"/>
-          <c:showVal val="1"/>
-          <c:showCatName val="0"/>
-          <c:showSerName val="0"/>
-          <c:showPercent val="0"/>
-          <c:showBubbleSize val="0"/>
-          <c:extLst>
-            <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
-          </c:extLst>
-        </c:dLbl>
-      </c:pivotFmt>
-      <c:pivotFmt>
-        <c:idx val="10"/>
-        <c:spPr>
-          <a:solidFill>
-            <a:schemeClr val="accent1">
-              <a:alpha val="85000"/>
-            </a:schemeClr>
-          </a:solidFill>
-          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-            <a:solidFill>
-              <a:schemeClr val="lt1">
-                <a:alpha val="50000"/>
-              </a:schemeClr>
-            </a:solidFill>
-            <a:round/>
-          </a:ln>
-          <a:effectLst/>
-        </c:spPr>
-        <c:dLbl>
-          <c:idx val="0"/>
-          <c:spPr>
-            <a:noFill/>
-            <a:ln>
-              <a:noFill/>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
-          <c:txPr>
-            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="overflow" horzOverflow="overflow" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
-              <a:spAutoFit/>
-            </a:bodyPr>
-            <a:lstStyle/>
-            <a:p>
-              <a:pPr>
-                <a:defRPr sz="1800" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-                  <a:solidFill>
-                    <a:schemeClr val="lt1"/>
-                  </a:solidFill>
-                  <a:latin typeface="+mn-lt"/>
-                  <a:ea typeface="+mn-ea"/>
-                  <a:cs typeface="+mn-cs"/>
-                </a:defRPr>
-              </a:pPr>
-              <a:endParaRPr lang="en-US"/>
-            </a:p>
-          </c:txPr>
-        </c:dLbl>
-      </c:pivotFmt>
-      <c:pivotFmt>
-        <c:idx val="11"/>
-        <c:spPr>
-          <a:solidFill>
-            <a:schemeClr val="accent1">
-              <a:alpha val="85000"/>
-            </a:schemeClr>
-          </a:solidFill>
-          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-            <a:solidFill>
-              <a:schemeClr val="lt1">
-                <a:alpha val="50000"/>
-              </a:schemeClr>
-            </a:solidFill>
-            <a:round/>
-          </a:ln>
-          <a:effectLst/>
-        </c:spPr>
-      </c:pivotFmt>
-      <c:pivotFmt>
-        <c:idx val="12"/>
-        <c:spPr>
-          <a:solidFill>
-            <a:schemeClr val="accent2">
-              <a:alpha val="85000"/>
-            </a:schemeClr>
-          </a:solidFill>
-          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-            <a:solidFill>
-              <a:schemeClr val="lt1">
-                <a:alpha val="50000"/>
-              </a:schemeClr>
-            </a:solidFill>
-            <a:round/>
-          </a:ln>
-          <a:effectLst/>
-        </c:spPr>
-        <c:dLbl>
-          <c:idx val="0"/>
-          <c:spPr>
-            <a:noFill/>
-            <a:ln>
-              <a:noFill/>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
-          <c:txPr>
-            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
-              <a:spAutoFit/>
-            </a:bodyPr>
-            <a:lstStyle/>
-            <a:p>
-              <a:pPr>
-                <a:defRPr sz="1800" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-                  <a:solidFill>
-                    <a:schemeClr val="lt1"/>
-                  </a:solidFill>
-                  <a:latin typeface="+mn-lt"/>
-                  <a:ea typeface="+mn-ea"/>
-                  <a:cs typeface="+mn-cs"/>
-                </a:defRPr>
-              </a:pPr>
-              <a:endParaRPr lang="en-US"/>
-            </a:p>
-          </c:txPr>
         </c:dLbl>
       </c:pivotFmt>
     </c:pivotFmts>
@@ -7416,7 +6572,7 @@
               <a:effectLst/>
             </c:spPr>
             <c:txPr>
-              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="overflow" horzOverflow="overflow" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
                 <a:spAutoFit/>
               </a:bodyPr>
               <a:lstStyle/>
@@ -8343,7 +7499,7 @@
         </c:dLbl>
       </c:pivotFmt>
       <c:pivotFmt>
-        <c:idx val="7"/>
+        <c:idx val="5"/>
         <c:spPr>
           <a:solidFill>
             <a:schemeClr val="accent1">
@@ -8361,19 +7517,7 @@
           <a:effectLst/>
         </c:spPr>
         <c:marker>
-          <c:symbol val="circle"/>
-          <c:size val="6"/>
-          <c:spPr>
-            <a:solidFill>
-              <a:schemeClr val="accent1">
-                <a:alpha val="85000"/>
-              </a:schemeClr>
-            </a:solidFill>
-            <a:ln>
-              <a:noFill/>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
+          <c:symbol val="none"/>
         </c:marker>
         <c:dLbl>
           <c:idx val="0"/>
@@ -8416,7 +7560,7 @@
         </c:dLbl>
       </c:pivotFmt>
       <c:pivotFmt>
-        <c:idx val="8"/>
+        <c:idx val="6"/>
         <c:spPr>
           <a:solidFill>
             <a:schemeClr val="accent1">
@@ -8434,19 +7578,7 @@
           <a:effectLst/>
         </c:spPr>
         <c:marker>
-          <c:symbol val="circle"/>
-          <c:size val="6"/>
-          <c:spPr>
-            <a:solidFill>
-              <a:schemeClr val="accent2">
-                <a:alpha val="85000"/>
-              </a:schemeClr>
-            </a:solidFill>
-            <a:ln>
-              <a:noFill/>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
+          <c:symbol val="none"/>
         </c:marker>
         <c:dLbl>
           <c:idx val="0"/>
@@ -13379,7 +12511,7 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="PivotChartTable4" cacheId="52" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="6" indent="0" multipleFieldFilters="0" chartFormat="2">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="PivotChartTable4" cacheId="3" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="6" indent="0" multipleFieldFilters="0" chartFormat="2">
   <location ref="A1:D10" firstHeaderRow="1" firstDataRow="2" firstDataCol="1"/>
   <pivotFields count="3">
     <pivotField dataField="1" showAll="0"/>
@@ -13450,7 +12582,7 @@
     <dataField name="Count of USPSANumber" fld="0" subtotal="count" baseField="0" baseItem="0"/>
   </dataFields>
   <chartFormats count="2">
-    <chartFormat chart="0" format="7" series="1">
+    <chartFormat chart="0" format="5" series="1">
       <pivotArea type="data" outline="0" fieldPosition="0">
         <references count="2">
           <reference field="4294967294" count="1" selected="0">
@@ -13462,7 +12594,7 @@
         </references>
       </pivotArea>
     </chartFormat>
-    <chartFormat chart="0" format="8" series="1">
+    <chartFormat chart="0" format="6" series="1">
       <pivotArea type="data" outline="0" fieldPosition="0">
         <references count="2">
           <reference field="4294967294" count="1" selected="0">
@@ -13628,7 +12760,7 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable2.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="PivotChartTable1" cacheId="23" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" chartFormat="3">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="PivotChartTable1" cacheId="1" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" chartFormat="3">
   <location ref="A1:B10" firstHeaderRow="1" firstDataRow="1" firstDataCol="1"/>
   <pivotFields count="2">
     <pivotField axis="axisRow" allDrilled="1" subtotalTop="0" showAll="0" sortType="descending" defaultAttributeDrillState="1">
@@ -13693,92 +12825,8 @@
   <dataFields count="1">
     <dataField name="Count of USPSANumber" fld="1" subtotal="count" baseField="0" baseItem="1"/>
   </dataFields>
-  <chartFormats count="8">
-    <chartFormat chart="0" format="19">
-      <pivotArea type="data" outline="0" fieldPosition="0">
-        <references count="2">
-          <reference field="4294967294" count="1" selected="0">
-            <x v="0"/>
-          </reference>
-          <reference field="0" count="1" selected="0">
-            <x v="5"/>
-          </reference>
-        </references>
-      </pivotArea>
-    </chartFormat>
-    <chartFormat chart="0" format="20">
-      <pivotArea type="data" outline="0" fieldPosition="0">
-        <references count="2">
-          <reference field="4294967294" count="1" selected="0">
-            <x v="0"/>
-          </reference>
-          <reference field="0" count="1" selected="0">
-            <x v="3"/>
-          </reference>
-        </references>
-      </pivotArea>
-    </chartFormat>
-    <chartFormat chart="0" format="21">
-      <pivotArea type="data" outline="0" fieldPosition="0">
-        <references count="2">
-          <reference field="4294967294" count="1" selected="0">
-            <x v="0"/>
-          </reference>
-          <reference field="0" count="1" selected="0">
-            <x v="7"/>
-          </reference>
-        </references>
-      </pivotArea>
-    </chartFormat>
-    <chartFormat chart="0" format="22">
-      <pivotArea type="data" outline="0" fieldPosition="0">
-        <references count="2">
-          <reference field="4294967294" count="1" selected="0">
-            <x v="0"/>
-          </reference>
-          <reference field="0" count="1" selected="0">
-            <x v="0"/>
-          </reference>
-        </references>
-      </pivotArea>
-    </chartFormat>
-    <chartFormat chart="0" format="23">
-      <pivotArea type="data" outline="0" fieldPosition="0">
-        <references count="2">
-          <reference field="4294967294" count="1" selected="0">
-            <x v="0"/>
-          </reference>
-          <reference field="0" count="1" selected="0">
-            <x v="2"/>
-          </reference>
-        </references>
-      </pivotArea>
-    </chartFormat>
-    <chartFormat chart="0" format="24">
-      <pivotArea type="data" outline="0" fieldPosition="0">
-        <references count="2">
-          <reference field="4294967294" count="1" selected="0">
-            <x v="0"/>
-          </reference>
-          <reference field="0" count="1" selected="0">
-            <x v="4"/>
-          </reference>
-        </references>
-      </pivotArea>
-    </chartFormat>
-    <chartFormat chart="0" format="25">
-      <pivotArea type="data" outline="0" fieldPosition="0">
-        <references count="2">
-          <reference field="4294967294" count="1" selected="0">
-            <x v="0"/>
-          </reference>
-          <reference field="0" count="1" selected="0">
-            <x v="6"/>
-          </reference>
-        </references>
-      </pivotArea>
-    </chartFormat>
-    <chartFormat chart="0" format="26" series="1">
+  <chartFormats count="1">
+    <chartFormat chart="0" format="37" series="1">
       <pivotArea type="data" outline="0" fieldPosition="0">
         <references count="1">
           <reference field="4294967294" count="1" selected="0">
@@ -13895,7 +12943,7 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable3.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="PivotChartTable2" cacheId="41" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" subtotalHiddenItems="1" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" chartFormat="3">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="PivotChartTable2" cacheId="2" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" subtotalHiddenItems="1" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" chartFormat="3">
   <location ref="A1:D3" firstHeaderRow="1" firstDataRow="2" firstDataCol="1"/>
   <pivotFields count="3">
     <pivotField allDrilled="1" subtotalTop="0" showAll="0" dataSourceSort="1" defaultAttributeDrillState="1">
@@ -13940,8 +12988,8 @@
       </extLst>
     </dataField>
   </dataFields>
-  <chartFormats count="3">
-    <chartFormat chart="0" format="10" series="1">
+  <chartFormats count="2">
+    <chartFormat chart="0" format="13" series="1">
       <pivotArea type="data" outline="0" fieldPosition="0">
         <references count="2">
           <reference field="4294967294" count="1" selected="0">
@@ -13953,19 +13001,7 @@
         </references>
       </pivotArea>
     </chartFormat>
-    <chartFormat chart="0" format="11">
-      <pivotArea type="data" outline="0" fieldPosition="0">
-        <references count="2">
-          <reference field="4294967294" count="1" selected="0">
-            <x v="0"/>
-          </reference>
-          <reference field="2" count="1" selected="0">
-            <x v="0"/>
-          </reference>
-        </references>
-      </pivotArea>
-    </chartFormat>
-    <chartFormat chart="0" format="12" series="1">
+    <chartFormat chart="0" format="14" series="1">
       <pivotArea type="data" outline="0" fieldPosition="0">
         <references count="2">
           <reference field="4294967294" count="1" selected="0">
@@ -14051,7 +13087,7 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable4.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="PivotChartTable3" cacheId="20" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="6" indent="0" multipleFieldFilters="0" chartFormat="2">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="PivotChartTable3" cacheId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="6" indent="0" multipleFieldFilters="0" chartFormat="2">
   <location ref="A1:A2" firstHeaderRow="1" firstDataRow="1" firstDataCol="0"/>
   <pivotFields count="1">
     <pivotField dataField="1" showAll="0"/>
@@ -39381,7 +38417,7 @@
   <dimension ref="A2:A10"/>
   <sheetViews>
     <sheetView zoomScale="112" zoomScaleNormal="126" workbookViewId="0">
-      <selection activeCell="L81" sqref="L81"/>
+      <selection activeCell="S35" sqref="S35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>

</xml_diff>